<commit_message>
Finalized presentation for 1/29 and added some pictures.
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88af51049543f108/Documents/A School Spring 2022/Project Lab/Project Lab 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88af51049543f108/Documents/A School Spring 2022/Project Lab/Project Lab 1/project-lab-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19A81015-E60A-4F7D-A3F7-4AB9A540454C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{19A81015-E60A-4F7D-A3F7-4AB9A540454C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2010EE8-25B5-4BDC-832C-EF724E2AA513}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>Erik Manis</t>
   </si>
   <si>
-    <t>Mohammed Santari</t>
-  </si>
-  <si>
     <t>DL Subtotal:</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>Mouser.com</t>
+  </si>
+  <si>
+    <t>Mohammed Ansari</t>
   </si>
 </sst>
 </file>
@@ -481,6 +481,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,10 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,30 +514,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -847,7 +847,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection sqref="A1:K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,16 +861,16 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
@@ -888,7 +888,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="4"/>
@@ -986,7 +986,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="B7" s="6">
         <v>15</v>
@@ -1020,11 +1020,11 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="16">
         <f>SUM(D5:D7)</f>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="8">
         <f>SUM(G5:G7)</f>
@@ -1041,10 +1041,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="9">
         <v>1</v>
@@ -1054,7 +1054,7 @@
         <v>1215</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="9">
         <v>1</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
@@ -1080,10 +1080,10 @@
         <f>SUM(G9:G10)</f>
         <v>6300</v>
       </c>
-      <c r="I11" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="33"/>
+      <c r="I11" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="35"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
@@ -1092,14 +1092,14 @@
       <c r="E12" s="6"/>
       <c r="F12" s="4"/>
       <c r="G12" s="7"/>
-      <c r="I12" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="30"/>
+      <c r="I12" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
@@ -1107,14 +1107,14 @@
       <c r="E13" s="6"/>
       <c r="F13" s="4"/>
       <c r="G13" s="7"/>
-      <c r="I13" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="28"/>
+      <c r="I13" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="39"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="6">
         <v>40</v>
@@ -1137,14 +1137,14 @@
         <f>E14*F14</f>
         <v>200</v>
       </c>
-      <c r="I14" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="32"/>
+      <c r="I14" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="6">
         <v>15</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="6">
         <v>200</v>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="4"/>
@@ -1276,34 +1276,34 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="K23" s="26"/>
+      <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="12">
         <f>449.99</f>
@@ -1327,18 +1327,18 @@
         <f>E24*F24*J24</f>
         <v>8.9998000000000005</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="34">
         <v>5</v>
       </c>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26">
+      <c r="I24" s="34"/>
+      <c r="J24" s="34">
         <v>10</v>
       </c>
-      <c r="K24" s="26"/>
+      <c r="K24" s="34"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="12">
         <f>415</f>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="4"/>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="4"/>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="9">
@@ -1428,11 +1428,11 @@
     </row>
     <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="19">
         <f>SUM(D28:D29)</f>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G30" s="5">
         <f>SUM(G28:G29)</f>
@@ -1473,7 +1473,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,30 +1483,30 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="34"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
@@ -1529,12 +1529,12 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="35">
+      <c r="J2" s="23">
         <f>SUM(B2:B30)</f>
         <v>27</v>
       </c>
@@ -1560,12 +1560,12 @@
       </c>
       <c r="G3" s="2"/>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="35">
+        <v>43</v>
+      </c>
+      <c r="J3" s="23">
         <f>SUM(C2:C30)</f>
         <v>27</v>
       </c>
@@ -1591,12 +1591,12 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="35">
+        <v>44</v>
+      </c>
+      <c r="J4" s="23">
         <f>SUM(D2:D30)</f>
         <v>27</v>
       </c>
@@ -1620,14 +1620,14 @@
       <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="35">
+      <c r="G5" s="24"/>
+      <c r="H5" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="23">
         <f>SUM(E2:E30)</f>
         <v>0</v>
       </c>
@@ -1653,12 +1653,12 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="35">
+        <v>45</v>
+      </c>
+      <c r="J6" s="23">
         <f>SUM(F2:F30)</f>
         <v>0</v>
       </c>
@@ -1684,12 +1684,12 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="35">
+        <v>20</v>
+      </c>
+      <c r="J7" s="23">
         <f>SUM(G2:G30)</f>
         <v>0</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1739,7 +1739,7 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1787,12 +1787,12 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="26"/>
+        <v>49</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
@@ -1814,13 +1814,13 @@
         <v>0</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="34"/>
+      <c r="H12" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="42"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="G13" s="2"/>
       <c r="H13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="G16" s="2"/>
       <c r="H16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1929,7 +1929,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1957,7 +1957,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1971,7 +1971,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1985,7 +1985,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1999,7 +1999,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2013,7 +2013,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2027,7 +2027,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2041,7 +2041,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2069,7 +2069,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2083,7 +2083,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2111,7 +2111,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2142,34 +2142,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="C1" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="27" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="1"/>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="41">
+        <v>59</v>
+      </c>
+      <c r="B2" s="29">
         <f>49.95</f>
         <v>49.95</v>
       </c>
@@ -2177,42 +2177,42 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="41">
+      <c r="F2" s="29">
         <f>B2*C2</f>
         <v>49.95</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="30">
         <f>SUM(F2:F21)</f>
         <v>224.86</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="41">
+        <v>60</v>
+      </c>
+      <c r="B3" s="29">
         <v>4.67</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="41">
+      <c r="F3" s="29">
         <f t="shared" ref="F3:F21" si="0">B3*C3</f>
         <v>4.67</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="41">
+        <v>62</v>
+      </c>
+      <c r="B4" s="29">
         <f>149</f>
         <v>149</v>
       </c>
@@ -2220,19 +2220,19 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="41">
+      <c r="F4" s="29">
         <f t="shared" si="0"/>
         <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="41">
+        <v>61</v>
+      </c>
+      <c r="B5" s="29">
         <f>3.3</f>
         <v>3.3</v>
       </c>
@@ -2241,16 +2241,16 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="41">
+      <c r="F5" s="29">
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="41">
+        <v>63</v>
+      </c>
+      <c r="B6" s="29">
         <f>3.95</f>
         <v>3.95</v>
       </c>
@@ -2258,19 +2258,19 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="41">
+      <c r="F6" s="29">
         <f t="shared" si="0"/>
         <v>3.95</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="41">
+        <v>64</v>
+      </c>
+      <c r="B7" s="29">
         <f>13.99</f>
         <v>13.99</v>
       </c>
@@ -2278,170 +2278,170 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="41">
+      <c r="F7" s="29">
         <f t="shared" si="0"/>
         <v>13.99</v>
       </c>
-      <c r="H7" s="39" t="s">
-        <v>41</v>
+      <c r="H7" s="27" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="41"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="41">
+      <c r="F8" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="40" t="s">
-        <v>42</v>
+      <c r="H8" s="28" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="41"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="41">
+      <c r="F9" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="41"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="41">
+      <c r="F10" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="41"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="41">
+      <c r="F11" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="41"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="41">
+      <c r="F12" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="41"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="41">
+      <c r="F13" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="41"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="41">
+      <c r="F14" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="41"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="41">
+      <c r="F15" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="41"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="41">
+      <c r="F16" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="41"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="41">
+      <c r="F17" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="41"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="41">
+      <c r="F18" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="41"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="41">
+      <c r="F19" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="41"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="41">
+      <c r="F20" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="41"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="41">
+      <c r="F21" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added a photo, updated the budget, and added Feb 2 Presentation.
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88af51049543f108/Documents/A School Spring 2022/Project Lab/Project Lab 1/project-lab-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edog3\OneDrive\Documents\A School Spring 2022\Project Lab\Project Lab 1\project-lab-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{19A81015-E60A-4F7D-A3F7-4AB9A540454C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2010EE8-25B5-4BDC-832C-EF724E2AA513}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88450D2D-C841-495B-A291-D4B806736363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" r:id="rId1"/>
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AB47C0-B6FA-4FC5-84F1-E15593E5DB37}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,11 +935,11 @@
       </c>
       <c r="C5" s="4">
         <f>'Labor Hours'!J2</f>
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D5" s="16">
         <f>B5*C5</f>
-        <v>405</v>
+        <v>585</v>
       </c>
       <c r="E5" s="6">
         <v>15</v>
@@ -967,11 +967,11 @@
       </c>
       <c r="C6" s="4">
         <f>'Labor Hours'!J3</f>
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D6" s="16">
         <f>B6*C6</f>
-        <v>405</v>
+        <v>585</v>
       </c>
       <c r="E6" s="6">
         <v>15</v>
@@ -993,11 +993,11 @@
       </c>
       <c r="C7" s="4">
         <f>'Labor Hours'!J4</f>
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D7" s="16">
         <f>B7*C7</f>
-        <v>405</v>
+        <v>540</v>
       </c>
       <c r="E7" s="6">
         <v>15</v>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="D9" s="16">
         <f>SUM(D5:D7)</f>
-        <v>1215</v>
+        <v>1710</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="4" t="s">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="D10" s="17">
         <f>D9</f>
-        <v>1215</v>
+        <v>1710</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>16</v>
@@ -1072,7 +1072,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="18">
         <f>SUM(D9:D10)</f>
-        <v>2430</v>
+        <v>3420</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="4"/>
@@ -1229,7 +1229,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="16">
         <f>'Material Costs'!H2</f>
-        <v>224.86</v>
+        <v>234.86</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="4"/>
@@ -1257,7 +1257,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="18">
         <f>D19</f>
-        <v>224.86</v>
+        <v>234.86</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="4"/>
@@ -1396,7 +1396,7 @@
       <c r="C28" s="4"/>
       <c r="D28" s="19">
         <f>SUM(D11,D17,D21,D26)</f>
-        <v>2663.5099</v>
+        <v>3663.5099</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="4"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="D29" s="17">
         <f>D28*C29</f>
-        <v>1198.5794550000001</v>
+        <v>1648.5794550000001</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="9">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="D30" s="19">
         <f>SUM(D28:D29)</f>
-        <v>3862.0893550000001</v>
+        <v>5312.0893550000001</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="15" t="s">
@@ -1472,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7020275-B2DA-4DA8-8538-10FD245A3C38}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,7 +1527,9 @@
       <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
       <c r="H2" t="s">
         <v>47</v>
       </c>
@@ -1536,7 +1538,7 @@
       </c>
       <c r="J2" s="23">
         <f>SUM(B2:B30)</f>
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1558,7 +1560,9 @@
       <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
       <c r="H3" t="s">
         <v>48</v>
       </c>
@@ -1567,7 +1571,7 @@
       </c>
       <c r="J3" s="23">
         <f>SUM(C2:C30)</f>
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1589,7 +1593,9 @@
       <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
       <c r="H4" t="s">
         <v>49</v>
       </c>
@@ -1598,7 +1604,7 @@
       </c>
       <c r="J4" s="23">
         <f>SUM(D2:D30)</f>
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1620,7 +1626,9 @@
       <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="24">
+        <v>0</v>
+      </c>
       <c r="H5" s="26" t="s">
         <v>50</v>
       </c>
@@ -1651,7 +1659,9 @@
       <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
       <c r="H6" t="s">
         <v>51</v>
       </c>
@@ -1682,7 +1692,9 @@
       <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
       <c r="H7" t="s">
         <v>52</v>
       </c>
@@ -1713,7 +1725,9 @@
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
       <c r="H8" t="s">
         <v>53</v>
       </c>
@@ -1737,7 +1751,9 @@
       <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
       <c r="H9" t="s">
         <v>47</v>
       </c>
@@ -1761,7 +1777,9 @@
       <c r="F10" s="2">
         <v>0</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
       <c r="H10" t="s">
         <v>48</v>
       </c>
@@ -1785,7 +1803,9 @@
       <c r="F11" s="2">
         <v>0</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
       <c r="H11" t="s">
         <v>49</v>
       </c>
@@ -1813,7 +1833,9 @@
       <c r="F12" s="2">
         <v>0</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
       <c r="H12" s="26" t="s">
         <v>50</v>
       </c>
@@ -1841,7 +1863,9 @@
       <c r="F13" s="2">
         <v>0</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
       <c r="H13" t="s">
         <v>51</v>
       </c>
@@ -1865,7 +1889,9 @@
       <c r="F14" s="2">
         <v>0</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
       <c r="H14" t="s">
         <v>52</v>
       </c>
@@ -1889,7 +1915,9 @@
       <c r="F15" s="2">
         <v>0</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
       <c r="H15" t="s">
         <v>53</v>
       </c>
@@ -1913,7 +1941,9 @@
       <c r="F16" s="2">
         <v>0</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
       <c r="H16" t="s">
         <v>47</v>
       </c>
@@ -1922,12 +1952,24 @@
       <c r="A17" s="20">
         <v>44588</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
       <c r="H17" t="s">
         <v>48</v>
       </c>
@@ -1936,12 +1978,24 @@
       <c r="A18" s="20">
         <v>44589</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
       <c r="H18" t="s">
         <v>49</v>
       </c>
@@ -1950,12 +2004,24 @@
       <c r="A19" s="20">
         <v>44590</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
       <c r="H19" s="14" t="s">
         <v>50</v>
       </c>
@@ -1964,12 +2030,24 @@
       <c r="A20" s="20">
         <v>44591</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
       <c r="H20" t="s">
         <v>51</v>
       </c>
@@ -1978,12 +2056,24 @@
       <c r="A21" s="20">
         <v>44592</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="B21" s="2">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
       <c r="H21" t="s">
         <v>52</v>
       </c>
@@ -1992,12 +2082,24 @@
       <c r="A22" s="20">
         <v>44593</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
       <c r="H22" t="s">
         <v>53</v>
       </c>
@@ -2006,12 +2108,24 @@
       <c r="A23" s="20">
         <v>44594</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="B23" s="2">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
       <c r="H23" t="s">
         <v>47</v>
       </c>
@@ -2130,7 +2244,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,7 +2300,7 @@
       </c>
       <c r="H2" s="30">
         <f>SUM(F2:F21)</f>
-        <v>224.86</v>
+        <v>234.86</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2233,8 +2347,8 @@
         <v>61</v>
       </c>
       <c r="B5" s="29">
-        <f>3.3</f>
-        <v>3.3</v>
+        <f>13.3</f>
+        <v>13.3</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -2243,7 +2357,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="29">
         <f t="shared" si="0"/>
-        <v>3.3</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
I updated the presentation for Feb 2 and added all of the photos for the presentation.
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edog3\OneDrive\Documents\A School Spring 2022\Project Lab\Project Lab 1\project-lab-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88af51049543f108/Documents/A School Spring 2022/Project Lab/Project Lab 1/project-lab-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88450D2D-C841-495B-A291-D4B806736363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{88450D2D-C841-495B-A291-D4B806736363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBE78A2C-65F4-47DD-AE42-EC1EDFCCF80E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8BB2A8C5-712E-4190-8588-7F5E0E3A700D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Budget" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
   <si>
     <t>Project Lab 1</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t>Mohammed Ansari</t>
+  </si>
+  <si>
+    <t>Power Supply</t>
+  </si>
+  <si>
+    <t>Soldering Iron</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,6 +535,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -844,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AB47C0-B6FA-4FC5-84F1-E15593E5DB37}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1323,7 @@
       </c>
       <c r="D24" s="17">
         <f>B24*C24*H24</f>
-        <v>4.4999000000000002</v>
+        <v>6.2998599999999998</v>
       </c>
       <c r="E24" s="12">
         <f>449.99</f>
@@ -1328,7 +1337,7 @@
         <v>8.9998000000000005</v>
       </c>
       <c r="H24" s="34">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I24" s="34"/>
       <c r="J24" s="34">
@@ -1349,7 +1358,7 @@
       </c>
       <c r="D25" s="17">
         <f>B25*C25*H24</f>
-        <v>4.1500000000000004</v>
+        <v>5.8100000000000005</v>
       </c>
       <c r="E25" s="12">
         <f>415</f>
@@ -1365,90 +1374,126 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="12">
+        <f>99.99</f>
+        <v>99.99</v>
+      </c>
+      <c r="C26" s="45">
+        <v>2E-3</v>
+      </c>
+      <c r="D26" s="10">
+        <f>B26*C26*H24</f>
+        <v>1.3998599999999999</v>
+      </c>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="12">
+        <f>99.99</f>
+        <v>99.99</v>
+      </c>
+      <c r="C27" s="13">
+        <v>2E-3</v>
+      </c>
+      <c r="D27" s="43">
+        <f>B27*C27*H24</f>
+        <v>1.3998599999999999</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="44"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="18">
-        <f>SUM(D24:D25)</f>
-        <v>8.6499000000000006</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="11">
+      <c r="B28" s="6"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="18">
+        <f>SUM(D24:D27)</f>
+        <v>14.909580000000002</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="11">
         <f>SUM(G24:G25)</f>
         <v>17.299800000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="6"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="19">
-        <f>SUM(D11,D17,D21,D26)</f>
-        <v>3663.5099</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="5">
-        <f>SUM(G11,G17,G21,G26)</f>
-        <v>8135.5097999999998</v>
-      </c>
-    </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
       <c r="B29" s="6"/>
-      <c r="C29" s="9">
-        <v>0.45</v>
-      </c>
-      <c r="D29" s="17">
-        <f>D28*C29</f>
-        <v>1648.5794550000001</v>
-      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="4"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="9">
-        <v>0.45</v>
-      </c>
-      <c r="G29" s="10">
-        <f>G28*F29</f>
-        <v>3660.9794099999999</v>
-      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="19">
+        <f>SUM(D11,D17,D21,D28)</f>
+        <v>3669.7695800000001</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5">
+        <f>SUM(G11,G17,G21,G28)</f>
+        <v>8135.5097999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="D31" s="17">
+        <f>D30*C31</f>
+        <v>1651.3963110000002</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="G31" s="10">
+        <f>G30*F31</f>
+        <v>3660.9794099999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="19">
-        <f>SUM(D28:D29)</f>
-        <v>5312.0893550000001</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="15" t="s">
+      <c r="D32" s="19">
+        <f>SUM(D30:D31)</f>
+        <v>5321.1658910000006</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="5">
-        <f>SUM(G28:G29)</f>
+      <c r="G32" s="5">
+        <f>SUM(G30:G31)</f>
         <v>11796.48921</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G32" s="4"/>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1472,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7020275-B2DA-4DA8-8538-10FD245A3C38}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,7 +2289,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>